<commit_message>
Choix par défaut pour les vols découvertes
 * Les listes déroulantes des noms et des avions affichent un
   champ vide par défaut.
 * Si la date du vol est inchangée, le fichier Excel ne sera pas
   rempli pour les champs pilote, avion, date, heure et temps.
 * Ajout des noms de pilote dans le fichier Excel

Signed-off-by: Gérard Parat <github@le-cycliste.fr>
</commit_message>
<xml_diff>
--- a/Gestion-VD.xlsx
+++ b/Gestion-VD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">GESTION DES VOLS DE DÉCOUVERTE</t>
   </si>
@@ -70,6 +70,9 @@
     <t xml:space="preserve">Autorisation parentale</t>
   </si>
   <si>
+    <t xml:space="preserve">John DOE</t>
+  </si>
+  <si>
     <t xml:space="preserve">F-OLIE</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">Chèque</t>
   </si>
   <si>
+    <t xml:space="preserve">Albert UNTEL</t>
+  </si>
+  <si>
     <t xml:space="preserve">F-RANC</t>
   </si>
   <si>
@@ -86,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Espèce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agathe ZEBLOUSE</t>
   </si>
   <si>
     <t xml:space="preserve">F-INAL</t>
@@ -655,14 +664,14 @@
   <dimension ref="A1:S155"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K9" activeCellId="0" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="30.7"/>
@@ -672,10 +681,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="4" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,14 +846,17 @@
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
       <c r="M9" s="35"/>
+      <c r="O9" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="P9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -860,14 +873,17 @@
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
       <c r="M10" s="35"/>
+      <c r="O10" s="0" t="s">
+        <v>20</v>
+      </c>
       <c r="P10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -884,11 +900,14 @@
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="35"/>
+      <c r="O11" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="P11" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -906,10 +925,10 @@
       <c r="L12" s="34"/>
       <c r="M12" s="35"/>
       <c r="P12" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3471,27 +3490,31 @@
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="H5:M5"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K7:K155" type="list">
+  <dataValidations count="5">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K7:K155" type="list">
       <formula1>$P$9:$P$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E155" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E155" type="list">
       <formula1>$S$9:$S$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L7:L155" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L155" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M7" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M7" type="list">
       <formula1>$Q$9:$Q$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L7" type="list">
+      <formula1>$O$9:$O$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>